<commit_message>
Update KDD Cup 2015 results
</commit_message>
<xml_diff>
--- a/KDD Cup 2015/kdd_cup_2015_results.xlsx
+++ b/KDD Cup 2015/kdd_cup_2015_results.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxva\Documents\Werk en stage\PhD\Dissertation\Learning Analytics\HITL Swarm\github\KDD Cup 2015\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86923B9-883D-4516-8308-2592C47351AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEADBD8-E69F-42B2-8CAE-BD6386F1783B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="FLAM" sheetId="5" r:id="rId2"/>
+    <sheet name="FLAME" sheetId="5" r:id="rId2"/>
     <sheet name="Regular" sheetId="2" r:id="rId3"/>
     <sheet name="Federated" sheetId="3" r:id="rId4"/>
     <sheet name="Local" sheetId="4" r:id="rId5"/>
@@ -135,9 +135,6 @@
     <t>Local</t>
   </si>
   <si>
-    <t>FLAM</t>
-  </si>
-  <si>
     <t>acc_nn</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>auc 10 clients</t>
+  </si>
+  <si>
+    <t>FLAME</t>
   </si>
 </sst>
 </file>
@@ -593,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -611,7 +611,7 @@
       <c r="A1" s="1"/>
       <c r="B1" s="9"/>
       <c r="C1" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="12" t="s">
@@ -637,7 +637,7 @@
         <v>20</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>23</v>
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C8368A-AED9-4872-8B7A-DD403DD96422}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -924,7 +924,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B3" s="5">
         <f>0.9/(1 + (Analysis!$H$3 - Analysis!$L$3))</f>
@@ -1004,13 +1004,13 @@
         <v>7</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>14</v>
@@ -1619,40 +1619,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -2064,40 +2064,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>